<commit_message>
Termino de reporte contribución
Se anexo el informe de excel en el cual representa cada uno de los contribuyentes
</commit_message>
<xml_diff>
--- a/Informes Y Presentaciones/Informe de contribuyentess.xlsx
+++ b/Informes Y Presentaciones/Informe de contribuyentess.xlsx
@@ -12,8 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet name="INFORME" sheetId="1" r:id="rId1"/>
-    <sheet name="DATA" sheetId="2" r:id="rId2"/>
+    <sheet name="INFORME CONTRIBUYENTES" sheetId="1" r:id="rId1"/>
+    <sheet name="DATA" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
-  <si>
-    <t>INFORME DE CONTRIBUYENTES</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>CONTRIBUYENTE</t>
   </si>
@@ -58,13 +55,52 @@
   </si>
   <si>
     <t>COMMITS</t>
+  </si>
+  <si>
+    <t>DATA DE CONTRIBUYENTES</t>
+  </si>
+  <si>
+    <t>DURACIÓN  PROYECTO</t>
+  </si>
+  <si>
+    <t>3 MESES</t>
+  </si>
+  <si>
+    <t>SEMANA 1</t>
+  </si>
+  <si>
+    <t>SEMANA 2</t>
+  </si>
+  <si>
+    <t>SEMANA 3</t>
+  </si>
+  <si>
+    <t>SEMANA 4</t>
+  </si>
+  <si>
+    <t>SEMANA 5</t>
+  </si>
+  <si>
+    <t>SEMANA 6</t>
+  </si>
+  <si>
+    <t>SEMANA 7</t>
+  </si>
+  <si>
+    <t>SEMANA 8</t>
+  </si>
+  <si>
+    <t>INFORME DE CONTRIBUYENTES PROYECTO CEDESOFT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,6 +110,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -101,7 +144,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -118,23 +161,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -152,20 +219,982 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:strRef>
+          <c:f>'INFORME CONTRIBUYENTES'!$C$12</c:f>
+          <c:strCache>
+            <c:ptCount val="1"/>
+            <c:pt idx="0">
+              <c:v>TENDENCIA DE CONTRIBUCIÓN JOSEPH PIZZA</c:v>
+            </c:pt>
+          </c:strCache>
+        </c:strRef>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="50" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:innerShdw blurRad="114300">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:innerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="8.1068697358807375E-3"/>
+                  <c:y val="-8.2033371932519394E-17"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.1068697358807375E-3"/>
+                  <c:y val="-4.4745992503109257E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-CO"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'INFORME CONTRIBUYENTES'!$F$23:$M$23</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>SEMANA 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SEMANA 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SEMANA 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>SEMANA 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SEMANA 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>SEMANA 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>SEMANA 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>SEMANA 8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'INFORME CONTRIBUYENTES'!$F$24:$M$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="445242064"/>
+        <c:axId val="445242456"/>
+      </c:areaChart>
+      <c:catAx>
+        <c:axId val="445242064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="445242456"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="445242456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="445242064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="284">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="20" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto">
+        <a:lumMod val="50000"/>
+      </cs:styleClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" b="1" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="74000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="74000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="70000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" cap="all" spc="50" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="15875" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" spc="20" baseline="0"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>171451</xdr:colOff>
+      <xdr:colOff>138320</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>35615</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>74064</xdr:colOff>
+      <xdr:colOff>42176</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>54665</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -188,14 +1217,44 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="638176" y="200025"/>
-          <a:ext cx="1912388" cy="1095375"/>
+          <a:off x="602146" y="217832"/>
+          <a:ext cx="1908247" cy="1095790"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>23811</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -464,56 +1523,150 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="21" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="3.7109375" customWidth="1"/>
-    <col min="5" max="5" width="3.85546875" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="3.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" customWidth="1"/>
+    <col min="4" max="4" width="2.140625" customWidth="1"/>
+    <col min="5" max="5" width="2.42578125" customWidth="1"/>
+    <col min="6" max="13" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:10" s="1" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="3:10" s="1" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="3:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
+    <row r="1" spans="3:15" s="1" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="3:15" s="1" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="3:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
     </row>
-    <row r="6" spans="3:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C10" s="3" t="s">
+    <row r="6" spans="3:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="4" t="s">
+    <row r="12" spans="3:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="9" t="str">
+        <f>+"TENDENCIA DE CONTRIBUCIÓN "&amp;C11</f>
+        <v>TENDENCIA DE CONTRIBUCIÓN JOSEPH PIZZA</v>
+      </c>
+    </row>
+    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C14" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="3">
+        <f>+VLOOKUP(C11,DATA!A:J,10,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="3:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C18" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C19" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="F23" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J23" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K23" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L23" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="M23" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="N23" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="F24" s="10">
+        <f>+VLOOKUP($C$11,DATA!$A$1:$J$8,MATCH('INFORME CONTRIBUYENTES'!F$23,DATA!$A$1:$J$1,0),0)</f>
+        <v>3</v>
+      </c>
+      <c r="G24" s="10">
+        <f>+VLOOKUP($C$11,DATA!$A$1:$J$8,MATCH('INFORME CONTRIBUYENTES'!G$23,DATA!$A$1:$J$1,0),0)</f>
+        <v>4</v>
+      </c>
+      <c r="H24" s="10">
+        <f>+VLOOKUP($C$11,DATA!$A$1:$J$8,MATCH('INFORME CONTRIBUYENTES'!H$23,DATA!$A$1:$J$1,0),0)</f>
+        <v>3</v>
+      </c>
+      <c r="I24" s="10">
+        <f>+VLOOKUP($C$11,DATA!$A$1:$J$8,MATCH('INFORME CONTRIBUYENTES'!I$23,DATA!$A$1:$J$1,0),0)</f>
+        <v>4</v>
+      </c>
+      <c r="J24" s="10">
+        <f>+VLOOKUP($C$11,DATA!$A$1:$J$8,MATCH('INFORME CONTRIBUYENTES'!J$23,DATA!$A$1:$J$1,0),0)</f>
         <v>2</v>
       </c>
+      <c r="K24" s="10">
+        <f>+VLOOKUP($C$11,DATA!$A$1:$J$8,MATCH('INFORME CONTRIBUYENTES'!K$23,DATA!$A$1:$J$1,0),0)</f>
+        <v>1</v>
+      </c>
+      <c r="L24" s="10">
+        <f>+VLOOKUP($C$11,DATA!$A$1:$J$8,MATCH('INFORME CONTRIBUYENTES'!L$23,DATA!$A$1:$J$1,0),0)</f>
+        <v>1</v>
+      </c>
+      <c r="M24" s="10">
+        <f>+VLOOKUP($C$11,DATA!$A$1:$J$8,MATCH('INFORME CONTRIBUYENTES'!M$23,DATA!$A$1:$J$1,0),0)</f>
+        <v>3</v>
+      </c>
+      <c r="N24" s="10">
+        <f>+VLOOKUP($C$11,DATA!$A$1:$J$8,MATCH('INFORME CONTRIBUYENTES'!N$23,DATA!$A$1:$J$1,0),0)</f>
+        <v>21</v>
+      </c>
     </row>
-    <row r="12" spans="3:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C14" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="5"/>
-    </row>
-    <row r="16" spans="3:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="F5:J5"/>
+    <mergeCell ref="F5:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -535,58 +1688,307 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:V8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B1" sqref="B1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="10.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8">
+        <f t="shared" ref="E1:V1" si="0">+U1+1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5">
         <v>3</v>
       </c>
+      <c r="C2" s="5">
+        <v>4</v>
+      </c>
+      <c r="D2" s="5">
+        <v>3</v>
+      </c>
+      <c r="E2" s="5">
+        <v>4</v>
+      </c>
+      <c r="F2" s="5">
+        <v>2</v>
+      </c>
+      <c r="G2" s="5">
+        <v>1</v>
+      </c>
+      <c r="H2" s="5">
+        <v>1</v>
+      </c>
+      <c r="I2" s="5">
+        <v>3</v>
+      </c>
+      <c r="J2" s="6">
+        <f>+SUM(B2:I2)</f>
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5">
+        <v>3</v>
+      </c>
+      <c r="G3" s="5">
         <v>2</v>
       </c>
+      <c r="H3" s="5">
+        <v>1</v>
+      </c>
+      <c r="I3" s="5">
+        <v>3</v>
+      </c>
+      <c r="J3" s="6">
+        <f t="shared" ref="J3:J8" si="1">+SUM(B3:I3)</f>
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
+      <c r="B4" s="5">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <v>2</v>
+      </c>
+      <c r="H4" s="5">
+        <v>2</v>
+      </c>
+      <c r="I4" s="5">
+        <v>2</v>
+      </c>
+      <c r="J4" s="6">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
+      <c r="B5" s="5">
+        <v>0</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="5">
+        <v>1</v>
+      </c>
+      <c r="I5" s="5">
+        <v>1</v>
+      </c>
+      <c r="J5" s="6">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0</v>
+      </c>
+      <c r="J6" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="B7" s="5">
+        <v>0</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5">
+        <v>1</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0</v>
+      </c>
+      <c r="I7" s="5">
+        <v>1</v>
+      </c>
+      <c r="J7" s="6">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
+      <c r="B8" s="5">
+        <f>+SUM(B2:B7)</f>
+        <v>3</v>
+      </c>
+      <c r="C8" s="5">
+        <f>+SUM(C2:C7)</f>
+        <v>5</v>
+      </c>
+      <c r="D8" s="5">
+        <f>+SUM(D2:D7)</f>
+        <v>3</v>
+      </c>
+      <c r="E8" s="5">
+        <f>+SUM(E2:E7)</f>
+        <v>5</v>
+      </c>
+      <c r="F8" s="5">
+        <f>+SUM(F2:F7)</f>
+        <v>6</v>
+      </c>
+      <c r="G8" s="5">
+        <f>+SUM(G2:G7)</f>
+        <v>5</v>
+      </c>
+      <c r="H8" s="5">
+        <f>+SUM(H2:H7)</f>
+        <v>5</v>
+      </c>
+      <c r="I8" s="5">
+        <f>+SUM(I2:I7)</f>
+        <v>10</v>
+      </c>
+      <c r="J8" s="6">
+        <f t="shared" si="1"/>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Presentaciones Y reportes de GITHUB
Final
</commit_message>
<xml_diff>
--- a/Informes Y Presentaciones/Informe de contribuyentess.xlsx
+++ b/Informes Y Presentaciones/Informe de contribuyentess.xlsx
@@ -235,13 +235,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -282,12 +282,11 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>TENDENCIA DE CONTRIBUCIÓN JOSEPH PIZZA</c:v>
+              <c:v>TENDENCIA DE CONTRIBUCIÓN TODOS LOS CONTRIBUYENTES</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -359,9 +358,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -379,9 +376,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -419,7 +414,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -479,25 +473,25 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -511,11 +505,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="364985584"/>
-        <c:axId val="364986368"/>
+        <c:axId val="373980232"/>
+        <c:axId val="287540952"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="364985584"/>
+        <c:axId val="373980232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -558,7 +552,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="364986368"/>
+        <c:crossAx val="287540952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -566,7 +560,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="364986368"/>
+        <c:axId val="287540952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -617,7 +611,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="364985584"/>
+        <c:crossAx val="373980232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -687,7 +681,7 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>FORMATO DE COMMITS JOSEPH PIZZA</c:v>
+              <c:v>FORMATO DE COMMITS JHON SEBASTIAN MONTOYA</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -908,16 +902,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>88</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2797,12 +2791,12 @@
   <sheetData>
     <row r="1" spans="11:14" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="11:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K4" s="12" t="s">
+      <c r="K4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
     </row>
     <row r="5" spans="11:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -2823,7 +2817,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="21" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2841,18 +2835,18 @@
     <row r="2" spans="3:15" s="1" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="3:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
     </row>
     <row r="6" spans="3:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="3:15" x14ac:dyDescent="0.25">
@@ -2862,13 +2856,13 @@
     </row>
     <row r="11" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="3" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="3:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C12" s="8" t="str">
         <f>+"TENDENCIA DE CONTRIBUCIÓN "&amp;C11</f>
-        <v>TENDENCIA DE CONTRIBUCIÓN JOSEPH PIZZA</v>
+        <v>TENDENCIA DE CONTRIBUCIÓN TODOS LOS CONTRIBUYENTES</v>
       </c>
     </row>
     <row r="14" spans="3:15" x14ac:dyDescent="0.25">
@@ -2879,7 +2873,7 @@
     <row r="15" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="3">
         <f>+VLOOKUP(C11,DATA!A:J,10,0)</f>
-        <v>21</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="3:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -2929,7 +2923,7 @@
       </c>
       <c r="G24" s="9">
         <f>+VLOOKUP($C$11,DATA!$A$1:$J$8,MATCH('INFORME CONTRIBUYENTES'!G$23,DATA!$A$1:$J$1,0),0)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H24" s="9">
         <f>+VLOOKUP($C$11,DATA!$A$1:$J$8,MATCH('INFORME CONTRIBUYENTES'!H$23,DATA!$A$1:$J$1,0),0)</f>
@@ -2937,27 +2931,27 @@
       </c>
       <c r="I24" s="9">
         <f>+VLOOKUP($C$11,DATA!$A$1:$J$8,MATCH('INFORME CONTRIBUYENTES'!I$23,DATA!$A$1:$J$1,0),0)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J24" s="9">
         <f>+VLOOKUP($C$11,DATA!$A$1:$J$8,MATCH('INFORME CONTRIBUYENTES'!J$23,DATA!$A$1:$J$1,0),0)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K24" s="9">
         <f>+VLOOKUP($C$11,DATA!$A$1:$J$8,MATCH('INFORME CONTRIBUYENTES'!K$23,DATA!$A$1:$J$1,0),0)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L24" s="9">
         <f>+VLOOKUP($C$11,DATA!$A$1:$J$8,MATCH('INFORME CONTRIBUYENTES'!L$23,DATA!$A$1:$J$1,0),0)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="M24" s="9">
         <f>+VLOOKUP($C$11,DATA!$A$1:$J$8,MATCH('INFORME CONTRIBUYENTES'!M$23,DATA!$A$1:$J$1,0),0)</f>
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="N24" s="9">
         <f>+VLOOKUP($C$11,DATA!$A$1:$J$8,MATCH('INFORME CONTRIBUYENTES'!N$23,DATA!$A$1:$J$1,0),0)</f>
-        <v>21</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -3010,18 +3004,18 @@
     <row r="2" spans="3:15" s="1" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="3:15" s="1" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
     </row>
     <row r="6" spans="3:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="3:15" x14ac:dyDescent="0.25">
@@ -3031,13 +3025,13 @@
     </row>
     <row r="9" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="3:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C10" s="8" t="str">
         <f>"FORMATO DE COMMITS "&amp;C9</f>
-        <v>FORMATO DE COMMITS JOSEPH PIZZA</v>
+        <v>FORMATO DE COMMITS JHON SEBASTIAN MONTOYA</v>
       </c>
     </row>
     <row r="11" spans="3:15" x14ac:dyDescent="0.25">
@@ -3048,7 +3042,7 @@
     <row r="12" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="3">
         <f>+VLOOKUP($C$11,DATA!$A$11:$H$15,MATCH('INFORME ARCHIVOS'!$C$9,DATA!$A$11:$H$11,0),0)</f>
-        <v>88</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="3:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -3060,7 +3054,7 @@
     <row r="15" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="3">
         <f>+VLOOKUP($C$14,DATA!$A$11:$H$15,MATCH('INFORME ARCHIVOS'!$C$9,DATA!$A$11:$H$11,0),0)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="3:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -3072,19 +3066,19 @@
     <row r="18" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="3">
         <f>+VLOOKUP($C$17,DATA!$A$11:$H$15,MATCH('INFORME ARCHIVOS'!$C$9,DATA!$A$11:$H$11,0),0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="3:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="10" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="21" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C21" s="3">
         <f>+VLOOKUP($C$20,DATA!$A$11:$H$15,MATCH('INFORME ARCHIVOS'!$C$9,DATA!$A$11:$H$11,0),0)</f>
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="3:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -3112,23 +3106,23 @@
     <row r="24" spans="3:14" x14ac:dyDescent="0.25">
       <c r="F24" s="9">
         <f>+VLOOKUP($C$9,DATA!$A$1:$J$8,MATCH('INFORME ARCHIVOS'!F$23,DATA!$A$1:$J$1,0),0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G24" s="9">
         <f>+C12</f>
-        <v>88</v>
+        <v>3</v>
       </c>
       <c r="H24" s="9">
         <f>+C15</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I24" s="9">
         <f>+C18</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J24" s="9">
         <f>+C21</f>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="K24" s="9"/>
       <c r="L24" s="9"/>
@@ -3144,7 +3138,7 @@
   <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATA!$A$2:$A$8</xm:f>
@@ -3161,8 +3155,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V15"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3246,11 +3241,11 @@
         <v>1</v>
       </c>
       <c r="I2" s="4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J2" s="5">
         <f>+SUM(B2:I2)</f>
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -3279,11 +3274,11 @@
         <v>1</v>
       </c>
       <c r="I3" s="4">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="J3" s="5">
         <f t="shared" ref="J3:J8" si="1">+SUM(B3:I3)</f>
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
@@ -3312,11 +3307,11 @@
         <v>2</v>
       </c>
       <c r="I4" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J4" s="5">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -3411,11 +3406,11 @@
         <v>0</v>
       </c>
       <c r="I7" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J7" s="5">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -3452,11 +3447,11 @@
       </c>
       <c r="I8" s="4">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="J8" s="5">
         <f t="shared" si="1"/>
-        <v>43</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
@@ -3517,10 +3512,10 @@
         <v>5</v>
       </c>
       <c r="C13" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D13" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E13" s="4">
         <v>2</v>
@@ -3532,8 +3527,8 @@
         <v>2</v>
       </c>
       <c r="H13" s="4">
-        <f t="shared" ref="H13:H16" si="3">+SUM(B13:G13)</f>
-        <v>12</v>
+        <f t="shared" ref="H13:H15" si="3">+SUM(B13:G13)</f>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
@@ -3574,7 +3569,7 @@
         <v>9</v>
       </c>
       <c r="D15" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E15" s="4">
         <v>3</v>
@@ -3583,11 +3578,11 @@
         <v>0</v>
       </c>
       <c r="G15" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H15" s="4">
         <f t="shared" si="3"/>
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>